<commit_message>
Changed the word "Faculty" to availability
</commit_message>
<xml_diff>
--- a/Visitor Preferences.xlsx
+++ b/Visitor Preferences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdowd\Documents\_Personal_Directory_\Personal_Files\Personal_Projects\ChemE Scheduling\ChemE-Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ED6621-166D-443D-9470-ADEDDD010A62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2080D2B9-B918-4869-9802-431421B5B2A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C747A6-EF44-496D-A099-BCB7F343D08D}"/>
   </bookViews>
@@ -56,6 +56,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{C85D6423-968E-4708-9C3E-72148E787745}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Garrett Dowdy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List the last names of the professors that each visitor is interested in meeting.  
+The names should be separated by a comma and a space.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -369,7 +394,7 @@
     <t>Availability</t>
   </si>
   <si>
-    <t>Preferred Faculty Meetings</t>
+    <t>Preferred Professor Meetings</t>
   </si>
 </sst>
 </file>
@@ -467,7 +492,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -539,7 +564,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -568,18 +593,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{732CC761-9082-47BF-884A-47DF1A8216B3}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{732CC761-9082-47BF-884A-47DF1A8216B3}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D33" xr:uid="{160A7554-00A7-4F75-95FF-80BCEA713474}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{18817D49-B3AF-4021-B7B2-44D4E2959568}" name="First Name" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{8031F382-7E80-4B0F-8CEF-EA5B2E88BC45}" name="Last Name" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{1D709BF6-DF01-429E-9FDE-3CC6381FD55A}" name="Availability" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5F8D594B-B601-47F6-8116-27697029A8A8}" name="Preferred Faculty Meetings" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{18817D49-B3AF-4021-B7B2-44D4E2959568}" name="First Name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8031F382-7E80-4B0F-8CEF-EA5B2E88BC45}" name="Last Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1D709BF6-DF01-429E-9FDE-3CC6381FD55A}" name="Availability" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5F8D594B-B601-47F6-8116-27697029A8A8}" name="Preferred Professor Meetings" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,7 +906,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>